<commit_message>
Apr 25 from office
</commit_message>
<xml_diff>
--- a/HLA2_reference alleles.xlsx
+++ b/HLA2_reference alleles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ys0/workbench/HLA_clustering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6994C43-6B52-044C-A10E-EF6D92BD6D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2B8936-7E79-E347-B513-140260E0BB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20340" yWindow="6060" windowWidth="28040" windowHeight="17440" xr2:uid="{17E6CD79-D2E9-FE4D-B87C-3906372D8EF0}"/>
+    <workbookView xWindow="19820" yWindow="14360" windowWidth="28040" windowHeight="17440" xr2:uid="{17E6CD79-D2E9-FE4D-B87C-3906372D8EF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="368">
   <si>
     <t>3lqz</t>
   </si>
@@ -1511,10 +1511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770C8809-59DD-B144-8754-14576FD34C1C}">
-  <dimension ref="A1:U157"/>
+  <dimension ref="A1:U313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53:U56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L288" sqref="L288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7309,7 +7309,7 @@
         <v>43257</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>98</v>
       </c>
@@ -7341,7 +7341,7 @@
         <v>43257</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>99</v>
       </c>
@@ -7373,7 +7373,7 @@
         <v>43257</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
         <v>100</v>
       </c>
@@ -7405,7 +7405,7 @@
         <v>43257</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <v>101</v>
       </c>
@@ -7437,7 +7437,7 @@
         <v>43691</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
         <v>102</v>
       </c>
@@ -7469,7 +7469,7 @@
         <v>43852</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>103</v>
       </c>
@@ -7499,7 +7499,7 @@
         <v>44160</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
         <v>104</v>
       </c>
@@ -7531,7 +7531,7 @@
         <v>44160</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <v>105</v>
       </c>
@@ -7563,7 +7563,7 @@
         <v>44160</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
         <v>106</v>
       </c>
@@ -7595,7 +7595,7 @@
         <v>44160</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>107</v>
       </c>
@@ -7625,7 +7625,7 @@
         <v>44160</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
         <v>108</v>
       </c>
@@ -7655,7 +7655,7 @@
         <v>44160</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
         <v>109</v>
       </c>
@@ -7685,7 +7685,7 @@
         <v>44160</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
         <v>110</v>
       </c>
@@ -7715,6 +7715,781 @@
       </c>
       <c r="J157" s="3">
         <v>44426</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L158" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L159" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L160" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="161" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L161" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="162" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L162" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="163" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L163" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="164" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L164" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="166" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L166" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="167" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L167" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="168" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L168" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="169" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L169" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="170" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L170" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="171" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L171" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="172" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L172" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="173" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L173" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="174" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L174" s="4">
+        <v>44685</v>
+      </c>
+    </row>
+    <row r="175" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L175" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="176" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L176" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="177" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L177" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="178" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L178" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="179" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L179" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="180" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L180" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="181" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L181" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="182" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L182" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="183" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L183" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="184" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L184" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="185" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L185" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="186" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L186" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="187" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L187" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="188" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L188" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="189" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L189" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="190" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L190" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="191" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L191" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="192" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L192" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="193" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L193" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="194" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L194" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="195" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L195" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="196" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L196" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="197" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L197" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="198" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L198" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="199" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L199" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="200" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L200" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="201" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L201" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="202" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L202" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="203" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L203" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="204" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L204" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="205" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L205" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="206" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L206" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="207" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L207" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="208" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L208" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="209" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L209" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="210" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L210" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="211" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L211" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="212" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L212" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="213" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L213" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="214" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L214" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="215" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L215" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="216" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L216" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="217" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L217" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="218" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L218" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="219" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L219" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="220" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L220" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="221" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L221" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="222" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L222" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="223" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L223" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="224" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L224" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="225" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L225" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="226" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L226" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="227" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L227" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="228" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L228" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="229" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L229" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="230" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L230" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="231" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L231" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="232" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L232" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="233" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L233" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="234" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L234" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="235" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L235" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="236" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L236" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="237" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L237" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="238" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L238" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="239" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L239" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="240" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L240" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="241" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L241" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="242" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L242" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="243" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L243" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="244" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L244" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="245" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L245" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="246" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L246" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="247" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L247" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="248" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L248" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="249" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L249" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="250" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L250" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="251" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L251" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="252" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L252" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="253" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L253" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="254" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L254" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="255" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L255" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="256" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L256" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="257" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L257" s="5">
+        <v>4E+41</v>
+      </c>
+    </row>
+    <row r="258" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L258" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="259" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L259" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="260" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L260" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="261" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L261" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="262" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L262" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="263" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L263" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="264" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L264" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="265" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L265" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="266" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L266" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="267" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L267" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="268" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L268" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="269" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L269" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="270" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L270" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="271" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L271" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="272" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L272" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="273" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L273" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="274" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L274" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="275" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L275" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="276" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L276" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="277" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L277" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="278" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L278" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="279" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L279" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="280" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L280" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="281" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L281" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="282" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L282" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="283" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L283" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="284" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L284" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="285" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L285" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="286" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L286" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="287" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L287" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="288" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L288" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="289" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L289" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="290" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L290" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="291" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L291" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="292" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L292" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="293" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L293" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="294" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L294" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="295" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L295" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="296" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L296" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="297" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L297" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="298" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L298" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="299" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L299" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="300" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L300" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="301" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L301" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="302" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L302" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="303" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L303" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="304" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L304" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="305" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L305" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="306" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L306" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="307" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L307" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="308" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L308" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="309" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L309" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="310" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L310" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="311" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L311" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="312" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L312" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="313" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L313" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -7918,6 +8693,161 @@
     <hyperlink ref="M54" r:id="rId197" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1H15" xr:uid="{C454A256-5A1D-6849-9C67-9343099B6212}"/>
     <hyperlink ref="M55" r:id="rId198" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1HQR" xr:uid="{3479DC39-1F67-C146-9396-42C3120D4A41}"/>
     <hyperlink ref="M56" r:id="rId199" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1ZGL" xr:uid="{E9200B7E-0A0B-D849-9E24-EF02DF827E70}"/>
+    <hyperlink ref="L158" r:id="rId200" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=3LQZ" xr:uid="{0E4AF2FE-E65F-B040-97CD-77626D694FB6}"/>
+    <hyperlink ref="L159" r:id="rId201" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=3WEX" xr:uid="{B18E577C-6561-3543-B799-FCFE0D2CEDE5}"/>
+    <hyperlink ref="L160" r:id="rId202" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4P4K" xr:uid="{D7DF6156-AA18-934B-9595-618E4FADC344}"/>
+    <hyperlink ref="L161" r:id="rId203" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4P4R" xr:uid="{25ADDF78-C21B-0E44-A76E-B8A8C482CE2F}"/>
+    <hyperlink ref="L162" r:id="rId204" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4P57" xr:uid="{5648F98E-E3CE-7F40-8359-D173C1F787E7}"/>
+    <hyperlink ref="L163" r:id="rId205" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4P5K" xr:uid="{45268941-D29E-2549-9A68-D38D23928D07}"/>
+    <hyperlink ref="L164" r:id="rId206" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4P5M" xr:uid="{10AAAD6F-1AD2-194C-9B46-223C3DA688B7}"/>
+    <hyperlink ref="L166" r:id="rId207" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1JK8" xr:uid="{CF171212-DC13-EB49-A5E1-5B6A2F2A31A5}"/>
+    <hyperlink ref="L167" r:id="rId208" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1S9V" xr:uid="{98EE9E2A-C3C8-7441-B153-563FF5388137}"/>
+    <hyperlink ref="L168" r:id="rId209" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1UVQ" xr:uid="{5FB1079E-39F3-E245-ACDB-6C370EF1505E}"/>
+    <hyperlink ref="L169" r:id="rId210" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=2NNA" xr:uid="{E8215394-5A7E-244D-A2DF-EF0A56C51E6F}"/>
+    <hyperlink ref="L170" r:id="rId211" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=3PL6" xr:uid="{F2CCE3E2-3DE2-D04A-94FF-28E292061665}"/>
+    <hyperlink ref="L171" r:id="rId212" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4D8P" xr:uid="{BEB56195-A726-3B4B-91B7-F73EACE91055}"/>
+    <hyperlink ref="L172" r:id="rId213" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4GG6" xr:uid="{1B5BB73B-A864-1248-9ECA-F3C2575A4C80}"/>
+    <hyperlink ref="L173" r:id="rId214" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4GRL" xr:uid="{D8332324-E7D1-5945-B162-EE590F23D465}"/>
+    <hyperlink ref="L174" r:id="rId215" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4MAY" xr:uid="{4D714268-5D1C-7A47-80AA-62C2D283DD48}"/>
+    <hyperlink ref="L175" r:id="rId216" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4OZF" xr:uid="{88AD0C78-6DE3-1A45-A77A-854B1FF23119}"/>
+    <hyperlink ref="L176" r:id="rId217" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4OZG" xr:uid="{2E287A5F-C2AF-9C4F-813A-372A6A74F4B0}"/>
+    <hyperlink ref="L177" r:id="rId218" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4OZH" xr:uid="{0E29DABC-A760-2649-8244-CF8D1404D52E}"/>
+    <hyperlink ref="L178" r:id="rId219" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4OZI" xr:uid="{8505D9A6-9D9C-D04B-8BB4-7114B96A75D8}"/>
+    <hyperlink ref="L179" r:id="rId220" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4Z7U" xr:uid="{9BE31ED1-423E-BC4C-A7B7-5A55E53054DB}"/>
+    <hyperlink ref="L180" r:id="rId221" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4Z7V" xr:uid="{7E5EAC57-16D6-D04F-BD56-5E27292E873C}"/>
+    <hyperlink ref="L181" r:id="rId222" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4Z7W" xr:uid="{B2F704E1-ED04-B445-955F-BAE988ECB347}"/>
+    <hyperlink ref="L182" r:id="rId223" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=5KS9" xr:uid="{21259562-B932-C14C-ABB6-F56FC618074E}"/>
+    <hyperlink ref="L183" r:id="rId224" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=5KSA" xr:uid="{D716011A-46A5-F04E-B3AA-F815193CD284}"/>
+    <hyperlink ref="L184" r:id="rId225" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=5KSB" xr:uid="{F57F75A0-1C8E-D044-BD77-DA5CED8267B9}"/>
+    <hyperlink ref="L185" r:id="rId226" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=5KSU" xr:uid="{1BCCA9A9-30EE-5A45-9F5A-D61FBE301071}"/>
+    <hyperlink ref="L186" r:id="rId227" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=5KSV" xr:uid="{02D6038D-7F13-A145-BC09-03B72BFDF7F4}"/>
+    <hyperlink ref="L187" r:id="rId228" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=5UJT" xr:uid="{B64D0310-2EB9-3142-86AA-E3FE32CF1B16}"/>
+    <hyperlink ref="L188" r:id="rId229" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6DFX" xr:uid="{7D47B782-C762-A44F-BA1D-CFE271B14ED9}"/>
+    <hyperlink ref="L189" r:id="rId230" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6DIG" xr:uid="{9E56C4A9-31BD-9A48-AACA-7096FF47FFAE}"/>
+    <hyperlink ref="L190" r:id="rId231" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6MFF" xr:uid="{5E765C91-1FBD-C948-8C35-A5B291177FFB}"/>
+    <hyperlink ref="L191" r:id="rId232" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6MFG" xr:uid="{909AE32F-668C-E845-A607-2CB039DF844D}"/>
+    <hyperlink ref="L192" r:id="rId233" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6PX6" xr:uid="{BF947210-E36B-3B46-A4BE-6F1F5EFBE09B}"/>
+    <hyperlink ref="L193" r:id="rId234" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6PY2" xr:uid="{7FA51B10-5022-8E45-98FB-251E214A8B03}"/>
+    <hyperlink ref="L194" r:id="rId235" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6U3M" xr:uid="{DFF69524-409D-9949-A951-C1719141FC56}"/>
+    <hyperlink ref="L195" r:id="rId236" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6U3N" xr:uid="{52C26810-487D-5544-8818-FEE14C4E500A}"/>
+    <hyperlink ref="L196" r:id="rId237" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6U3O" xr:uid="{2B1D886A-D445-1C47-97DF-1A300ED5B63A}"/>
+    <hyperlink ref="L197" r:id="rId238" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6XC9" xr:uid="{FAE74D20-D395-354C-B696-8627EF16BA95}"/>
+    <hyperlink ref="L198" r:id="rId239" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6XCO" xr:uid="{8719AC8F-D5A4-1E4F-A9A9-1698F33662DD}"/>
+    <hyperlink ref="L199" r:id="rId240" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6XCP" xr:uid="{101A7F0A-8D6B-7A4B-A5D6-DB14FDBBF7D8}"/>
+    <hyperlink ref="L200" r:id="rId241" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6XP6" xr:uid="{20B0062A-E075-434A-AEE9-9D5A55DEB90E}"/>
+    <hyperlink ref="L201" r:id="rId242" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=7KEI" xr:uid="{FC6B58EA-025B-E845-9C97-ACAFD8BE9619}"/>
+    <hyperlink ref="L202" r:id="rId243" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1A6A" xr:uid="{BEBDC39B-F500-D34A-A186-40E29243FDD7}"/>
+    <hyperlink ref="L203" r:id="rId244" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1AQD" xr:uid="{54221763-8E52-574F-872B-8545825D0C56}"/>
+    <hyperlink ref="L204" r:id="rId245" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1BX2" xr:uid="{DFCFEDCA-79B5-3548-BD6D-CD286946A702}"/>
+    <hyperlink ref="L205" r:id="rId246" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1D5M" xr:uid="{CBE2FA70-5636-6340-B7D9-91F4BFC479A6}"/>
+    <hyperlink ref="L206" r:id="rId247" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1D5X" xr:uid="{DAC9E65A-1A27-2D4D-B865-77EE352791AF}"/>
+    <hyperlink ref="L207" r:id="rId248" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1D5Z" xr:uid="{CD2E1F46-1D15-8A46-9E86-F634B0A3A881}"/>
+    <hyperlink ref="L208" r:id="rId249" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1D6E" xr:uid="{922D4E55-8C56-654D-AF30-7B279E985006}"/>
+    <hyperlink ref="L209" r:id="rId250" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1DLH" xr:uid="{D30F1C45-81CC-2B4B-A709-C1261BBBE066}"/>
+    <hyperlink ref="L210" r:id="rId251" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1FV1" xr:uid="{53EE1B42-6A0D-A548-BA3C-BBAD56863BC2}"/>
+    <hyperlink ref="L211" r:id="rId252" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1FYT" xr:uid="{1E276F18-12F0-B247-A3C8-2E10102B7E4C}"/>
+    <hyperlink ref="L212" r:id="rId253" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1H15" xr:uid="{3CE703E5-0030-DB4A-B9CD-0990F15CD5B8}"/>
+    <hyperlink ref="L213" r:id="rId254" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1HQR" xr:uid="{51C3763C-CEC2-F347-B1ED-CAC8C8DDD906}"/>
+    <hyperlink ref="L214" r:id="rId255" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1HXY" xr:uid="{0F48D61E-6311-0246-A316-6F20726D0E68}"/>
+    <hyperlink ref="L215" r:id="rId256" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1J8H" xr:uid="{59BD0B07-DA90-694C-8019-67DA94C59B5C}"/>
+    <hyperlink ref="L216" r:id="rId257" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1JWM" xr:uid="{36DC5947-E8EA-2244-AE9F-DFCBB8BDA9DA}"/>
+    <hyperlink ref="L217" r:id="rId258" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1JWS" xr:uid="{A5D16B88-F9FE-914B-9AED-9C4A78CD17F5}"/>
+    <hyperlink ref="L218" r:id="rId259" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1JWU" xr:uid="{3A19C3E9-9456-5E48-B692-F6608F14E3F3}"/>
+    <hyperlink ref="L219" r:id="rId260" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1KG0" xr:uid="{A50947BF-751B-5247-81D0-AC0E1B31646B}"/>
+    <hyperlink ref="L220" r:id="rId261" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1KLG" xr:uid="{8B9C23BB-9BD6-3547-988B-9BBA7620F406}"/>
+    <hyperlink ref="L221" r:id="rId262" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1KLU" xr:uid="{048274B3-7789-3F4B-A61E-5716288BF8E3}"/>
+    <hyperlink ref="L222" r:id="rId263" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1LO5" xr:uid="{A8B0EE20-DAE9-9643-8523-45BE0AD66F71}"/>
+    <hyperlink ref="L223" r:id="rId264" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1PYW" xr:uid="{C599EFA9-44CA-8C4F-AFC8-93158FC0D67F}"/>
+    <hyperlink ref="L224" r:id="rId265" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1R5I" xr:uid="{A02BB483-DEF7-064E-9D67-556E8F0C174F}"/>
+    <hyperlink ref="L225" r:id="rId266" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1SEB" xr:uid="{218E3F70-60AD-3040-9C51-DB7872371AD1}"/>
+    <hyperlink ref="L226" r:id="rId267" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1SJE" xr:uid="{9DD3C5A7-AD82-1141-8398-0014DEA870F8}"/>
+    <hyperlink ref="L227" r:id="rId268" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1SJH" xr:uid="{D9B38844-8ACD-484E-9C89-3838E09F77A7}"/>
+    <hyperlink ref="L228" r:id="rId269" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1T5W" xr:uid="{F3A1F421-3646-AE40-A4EC-D662D80AA64C}"/>
+    <hyperlink ref="L229" r:id="rId270" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1T5X" xr:uid="{6E76960A-1D0C-E243-BCDD-2E0C28FE9490}"/>
+    <hyperlink ref="L230" r:id="rId271" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1YMM" xr:uid="{4667FA1E-B334-F34F-BB02-ACDFA843FB6D}"/>
+    <hyperlink ref="L231" r:id="rId272" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=1ZGL" xr:uid="{1090A9CE-8154-5848-9316-4CC62E732516}"/>
+    <hyperlink ref="L232" r:id="rId273" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=2FSE" xr:uid="{3AEB05E7-0A2D-EF49-93FF-D75F0FB64B6E}"/>
+    <hyperlink ref="L233" r:id="rId274" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=2G9H" xr:uid="{94AE6264-ECCA-3243-932C-EFF36BAC16D8}"/>
+    <hyperlink ref="L234" r:id="rId275" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=2IAM" xr:uid="{2B0350E3-4DF4-AF46-9917-4F1D50330139}"/>
+    <hyperlink ref="L235" r:id="rId276" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=2IAN" xr:uid="{4FCAEF6B-B3FF-744F-B76C-3DFA63BF751C}"/>
+    <hyperlink ref="L236" r:id="rId277" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=2ICW" xr:uid="{A9C542BD-454C-6A4F-8A98-F8B67CEDD988}"/>
+    <hyperlink ref="L237" r:id="rId278" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=2IPK" xr:uid="{DF6556DD-EBD2-CA40-8714-A57894A5C36E}"/>
+    <hyperlink ref="L238" r:id="rId279" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=2OJE" xr:uid="{5E26A473-0821-D844-93DF-F99DCBFCD771}"/>
+    <hyperlink ref="L239" r:id="rId280" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=2Q6W" xr:uid="{B3EE346C-95F2-494E-9985-EBCA469C2FE8}"/>
+    <hyperlink ref="L240" r:id="rId281" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=2SEB" xr:uid="{22E0A5A3-F815-4B49-8450-03D4D155072C}"/>
+    <hyperlink ref="L241" r:id="rId282" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=2WBJ" xr:uid="{9DD9E498-7B8B-F44C-9B3A-CB1EBE28CE4C}"/>
+    <hyperlink ref="L242" r:id="rId283" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=2XN9" xr:uid="{932447E5-FCE3-2945-A5F0-D0A897FF35C3}"/>
+    <hyperlink ref="L243" r:id="rId284" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=3C5J" xr:uid="{52DAA4A0-7541-8843-9D86-B52D4650ABBD}"/>
+    <hyperlink ref="L244" r:id="rId285" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=3L6F" xr:uid="{338F8D0E-07BF-D54D-BD08-608F9099DDF5}"/>
+    <hyperlink ref="L245" r:id="rId286" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=3O6F" xr:uid="{C4148E90-CB7E-244B-89A9-28BEB5C23C52}"/>
+    <hyperlink ref="L246" r:id="rId287" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=3PDO" xr:uid="{68DB2EC2-9A5D-2543-A82C-B29BA82BB76E}"/>
+    <hyperlink ref="L247" r:id="rId288" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=3PGC" xr:uid="{7DA2E70A-A7ED-F142-8F10-B631BDFC1D73}"/>
+    <hyperlink ref="L248" r:id="rId289" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=3PGD" xr:uid="{1CEBE9EC-5DC0-8246-9DA3-71D702F86869}"/>
+    <hyperlink ref="L249" r:id="rId290" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=3QXA" xr:uid="{2CBC5DA9-7E14-5E4C-B276-3F17C43F88D5}"/>
+    <hyperlink ref="L250" r:id="rId291" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=3QXD" xr:uid="{628711EA-E444-3445-A44A-FA984920DD18}"/>
+    <hyperlink ref="L251" r:id="rId292" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=3S4S" xr:uid="{78171AF0-499A-4C4A-8AE5-D438AE122FC8}"/>
+    <hyperlink ref="L252" r:id="rId293" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=3S5L" xr:uid="{B86FAA6E-9C1D-E948-9DB6-B05295772E49}"/>
+    <hyperlink ref="L253" r:id="rId294" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=3T0E" xr:uid="{F1CAE00A-81CB-5841-AD7F-72218D4855C3}"/>
+    <hyperlink ref="L254" r:id="rId295" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4AEN" xr:uid="{5F1EF87D-E58E-5F4A-B0DE-28D56E42BCFF}"/>
+    <hyperlink ref="L255" r:id="rId296" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4AH2" xr:uid="{B752A7E7-EF66-8C4C-8694-2578B1D2C112}"/>
+    <hyperlink ref="L256" r:id="rId297" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4C56" xr:uid="{32B0BBB3-1847-3B48-A69E-AD484689C233}"/>
+    <hyperlink ref="L257" r:id="rId298" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4E41" xr:uid="{3F5B0712-F23B-4247-8852-A2F9D7283C4F}"/>
+    <hyperlink ref="L258" r:id="rId299" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4FQX" xr:uid="{BF0E63B6-C634-794C-947B-A359DF26FFB6}"/>
+    <hyperlink ref="L259" r:id="rId300" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4GBX" xr:uid="{DB963D1F-0E11-B14F-AB96-0F4C1F6E385A}"/>
+    <hyperlink ref="L260" r:id="rId301" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4H1L" xr:uid="{8B0FDF70-C71A-C14E-83F4-52951C20B1C6}"/>
+    <hyperlink ref="L261" r:id="rId302" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4H25" xr:uid="{A0A74BCD-4B96-1A4E-A8EC-1F182E5D7C97}"/>
+    <hyperlink ref="L262" r:id="rId303" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4H26" xr:uid="{02DF9727-6BA4-F940-9779-913B23CBA8AF}"/>
+    <hyperlink ref="L263" r:id="rId304" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4I5B" xr:uid="{D6D4667F-AB94-874E-91EF-10EA396C7EBA}"/>
+    <hyperlink ref="L264" r:id="rId305" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4IS6" xr:uid="{BCDA5B1C-B260-D441-AB27-D56BC65251C2}"/>
+    <hyperlink ref="L265" r:id="rId306" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4MCY" xr:uid="{099B19C1-534A-2E45-AAF5-C0D627F1B3E5}"/>
+    <hyperlink ref="L266" r:id="rId307" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4MCZ" xr:uid="{85AA0589-1E60-2B43-AEEB-81E5712245B3}"/>
+    <hyperlink ref="L267" r:id="rId308" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4MD0" xr:uid="{61F7266D-364F-6649-A794-532037AA6D89}"/>
+    <hyperlink ref="L268" r:id="rId309" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4MD4" xr:uid="{259C118C-2787-0A42-A508-15A0F5674CEA}"/>
+    <hyperlink ref="L269" r:id="rId310" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4MD5" xr:uid="{AC6ECA58-DCCF-A744-832E-9667A9121D53}"/>
+    <hyperlink ref="L270" r:id="rId311" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4MDI" xr:uid="{05007D3E-97F7-3040-82C8-8692F9177DD0}"/>
+    <hyperlink ref="L271" r:id="rId312" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4MDJ" xr:uid="{5A695830-5431-8F45-84CF-CE1C78A2B0D5}"/>
+    <hyperlink ref="L272" r:id="rId313" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4OV5" xr:uid="{418B7BDF-2F90-7248-918B-E0A147EA007F}"/>
+    <hyperlink ref="L273" r:id="rId314" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4X5W" xr:uid="{1ED317B4-F63A-B64D-8E82-F2D00485E413}"/>
+    <hyperlink ref="L274" r:id="rId315" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4X5X" xr:uid="{385739B7-AD6A-1748-8E78-70B6857A9ED8}"/>
+    <hyperlink ref="L275" r:id="rId316" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4Y19" xr:uid="{17082E2F-0C07-A445-85DA-664BA8C009AE}"/>
+    <hyperlink ref="L276" r:id="rId317" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=4Y1A" xr:uid="{9E5C97B0-B17F-464B-97F9-42A00D888416}"/>
+    <hyperlink ref="L277" r:id="rId318" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=5JLZ" xr:uid="{CC1AD382-05E6-A340-987B-329989621E26}"/>
+    <hyperlink ref="L278" r:id="rId319" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=5LAX" xr:uid="{86BDC627-9F19-7747-9B34-2A9FEC3ED9CF}"/>
+    <hyperlink ref="L279" r:id="rId320" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=5NI9" xr:uid="{88D9C4D6-83D8-D343-83F6-B351738837D1}"/>
+    <hyperlink ref="L280" r:id="rId321" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=5NIG" xr:uid="{44BFEED1-2FDE-0344-8B3B-8AFF0C82CB1A}"/>
+    <hyperlink ref="L281" r:id="rId322" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=5V4M" xr:uid="{00049880-9F66-AB45-B824-7F8A05EF5004}"/>
+    <hyperlink ref="L282" r:id="rId323" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=5V4N" xr:uid="{528E750C-D0A8-784C-A194-0D001B1961A0}"/>
+    <hyperlink ref="L283" r:id="rId324" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6ATF" xr:uid="{08C06AC8-8553-4846-95EB-F710D97AA092}"/>
+    <hyperlink ref="L284" r:id="rId325" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6ATI" xr:uid="{F79EECA5-663F-2747-AA18-612450F6FF88}"/>
+    <hyperlink ref="L285" r:id="rId326" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6ATZ" xr:uid="{4432DC1C-9D56-3A48-A302-41732447E9BF}"/>
+    <hyperlink ref="L286" r:id="rId327" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6BIJ" xr:uid="{5FA56B88-5FB3-1245-AD9E-24D5EC732D5C}"/>
+    <hyperlink ref="L287" r:id="rId328" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6BIL" xr:uid="{B312C4A8-F360-B146-A673-F2DC91704B6A}"/>
+    <hyperlink ref="L288" r:id="rId329" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6BIN" xr:uid="{11415264-2200-9B46-8A79-3B5569523832}"/>
+    <hyperlink ref="L289" r:id="rId330" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6BIR" xr:uid="{AA4DBBEF-11E1-7343-BCBA-7AB66F4E644F}"/>
+    <hyperlink ref="L290" r:id="rId331" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6BIV" xr:uid="{6582EAA2-D911-FD44-8B1F-CAE554F6E132}"/>
+    <hyperlink ref="L291" r:id="rId332" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6BIX" xr:uid="{13C4E0F6-77C5-A84F-9633-648140B04034}"/>
+    <hyperlink ref="L292" r:id="rId333" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6BIY" xr:uid="{9C94DA4C-EFBC-1849-82BC-EAF72DACDA61}"/>
+    <hyperlink ref="L293" r:id="rId334" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6BIZ" xr:uid="{48463EAE-5348-FC4D-BC77-3F3DD119A011}"/>
+    <hyperlink ref="L294" r:id="rId335" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6CPL" xr:uid="{22C69BB5-4233-6F4B-8D1D-F2F3A08024E9}"/>
+    <hyperlink ref="L295" r:id="rId336" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6CPN" xr:uid="{97218735-5F87-584C-B544-A855404A8F92}"/>
+    <hyperlink ref="L296" r:id="rId337" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6CPO" xr:uid="{A0B545EF-DE7F-7143-BE3C-405AC6C7E019}"/>
+    <hyperlink ref="L297" r:id="rId338" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6CQJ" xr:uid="{B5106F02-3DFE-9B4E-B650-7066E0C400FD}"/>
+    <hyperlink ref="L298" r:id="rId339" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6CQL" xr:uid="{6A81DDD1-4115-254D-8A35-78E52B6EBF50}"/>
+    <hyperlink ref="L299" r:id="rId340" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6CQN" xr:uid="{84D10B6C-8D0B-2D43-AE10-A70BB780A717}"/>
+    <hyperlink ref="L300" r:id="rId341" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6CQQ" xr:uid="{8F768BB5-213A-104F-88E4-08CE95DDE509}"/>
+    <hyperlink ref="L301" r:id="rId342" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6CQR" xr:uid="{0DEFF247-2E81-F04A-BED4-6112A1728B3D}"/>
+    <hyperlink ref="L302" r:id="rId343" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6HBY" xr:uid="{E0BB5E71-DD58-734F-908C-CD87EFE853D9}"/>
+    <hyperlink ref="L303" r:id="rId344" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6NIX" xr:uid="{C022CD45-1CBE-8340-A669-3667A54320FE}"/>
+    <hyperlink ref="L304" r:id="rId345" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6T3Y" xr:uid="{1C04F7A1-774E-5549-9D72-AAE6FD1DFBB6}"/>
+    <hyperlink ref="L305" r:id="rId346" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6V0Y" xr:uid="{4D2397E5-6896-E84A-9D88-FD9930D55568}"/>
+    <hyperlink ref="L306" r:id="rId347" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6V13" xr:uid="{82159D1A-6E1B-E24B-8203-0D0B6CE6B010}"/>
+    <hyperlink ref="L307" r:id="rId348" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6V15" xr:uid="{5BD47D7D-2D86-FC43-84E0-1FE5FA2092B7}"/>
+    <hyperlink ref="L308" r:id="rId349" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6V18" xr:uid="{028E6908-A1D8-D248-9097-6DE62D9ABD58}"/>
+    <hyperlink ref="L309" r:id="rId350" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6V19" xr:uid="{A1503BA0-0FE1-404B-B113-2E23854C0BC7}"/>
+    <hyperlink ref="L310" r:id="rId351" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6V1A" xr:uid="{75493C73-B2C4-8E42-9DCE-3E3EB7F89F28}"/>
+    <hyperlink ref="L311" r:id="rId352" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=7N19" xr:uid="{751721E6-30EC-F940-8882-64F350E5DA34}"/>
+    <hyperlink ref="L312" r:id="rId353" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6DFS" xr:uid="{90FB63CA-8B1F-9746-B8C9-DC3D46BE1C79}"/>
+    <hyperlink ref="L313" r:id="rId354" display="https://www.imgt.org/3Dstructure-DB/cgi/details.cgi?pdbcode=6DFW" xr:uid="{69103412-2DFC-C446-BB43-19DFD43A67B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>